<commit_message>
Módulo 13 - Ferramenta de Análises (solver)
</commit_message>
<xml_diff>
--- a/Módulo 13 - Analise de dados/aula-solver.xlsx
+++ b/Módulo 13 - Analise de dados/aula-solver.xlsx
@@ -1,60 +1,107 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Google Drive\Curso_Excel\12 Ferramentas de análise\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Curso Excel do básico ao avançado\Módulo 13 - Analise de dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEA3781-17DD-4436-B76E-0EB86D36D0CA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4430C8C5-1BA6-4289-86B7-BC19EE26AF37}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10485" windowHeight="7470" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Solver" sheetId="2" r:id="rId1"/>
+    <sheet name="Solver (2)" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Solver!$C$6:$C$9</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">'Solver (2)'!$C$6:$C$9</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">Solver!$C$6:$C$9</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'Solver (2)'!$C$6:$C$9</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">Solver!$C$6:$C$9</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Solver!$F$11:$H$11</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">'Solver (2)'!$C$6:$C$9</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Solver!$C$7</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">'Solver (2)'!$C$7</definedName>
     <definedName name="solver_lhs4" localSheetId="0" hidden="1">Solver!$F$11:$H$11</definedName>
+    <definedName name="solver_lhs4" localSheetId="1" hidden="1">'Solver (2)'!$F$11:$H$11</definedName>
+    <definedName name="solver_lhs5" localSheetId="0" hidden="1">Solver!$F$11:$H$11</definedName>
+    <definedName name="solver_lhs5" localSheetId="1" hidden="1">'Solver (2)'!$F$11:$H$11</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">4</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">4</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Solver!$B$12</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">'Solver (2)'!$B$12</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">4</definedName>
+    <definedName name="solver_rel2" localSheetId="1" hidden="1">4</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel3" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel4" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel5" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel5" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">Solver!$E$6:$E$9</definedName>
-    <definedName name="solver_rhs2" localSheetId="0" hidden="1">número inteiro</definedName>
-    <definedName name="solver_rhs3" localSheetId="0" hidden="1">Solver!$F$12:$H$12</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">'Solver (2)'!$E$6:$E$9</definedName>
+    <definedName name="solver_rhs2" localSheetId="0" hidden="1">"número inteiro"</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">"número inteiro"</definedName>
+    <definedName name="solver_rhs3" localSheetId="0" hidden="1">Solver!$E$7</definedName>
+    <definedName name="solver_rhs3" localSheetId="1" hidden="1">'Solver (2)'!$E$7</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">Solver!$F$12:$H$12</definedName>
+    <definedName name="solver_rhs4" localSheetId="1" hidden="1">'Solver (2)'!$F$12:$H$12</definedName>
+    <definedName name="solver_rhs5" localSheetId="0" hidden="1">Solver!$F$12:$H$12</definedName>
+    <definedName name="solver_rhs5" localSheetId="1" hidden="1">'Solver (2)'!$F$12:$H$12</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -64,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
   <si>
     <r>
       <t xml:space="preserve">EducandoWeb
@@ -126,11 +173,87 @@
   <si>
     <t>PLANO MENSAL DE PRODUÇÃO</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Questão de negócio:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> dadas as restrições de demanda de mercado e de produção, quantas unidades de cada produto eu devo produzir para maximizar meu lucro mensal?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Aplicabilidade: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>é uma ferramenta usada para obter soluções ótimas(minimo e máximo), ou metas, dado um conjunto de variáveis e restrições.</t>
+    </r>
+  </si>
+  <si>
+    <t>somarProduto</t>
+  </si>
+  <si>
+    <t>Manual</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Solver - Criação:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Dados/Solver/aba de parâmetros/Define o objetivo(lucro)/Seleciona a variável que deseja(max-min-valor)/
+Adiciona as restrições: Adicionar/nova aba insere: referencia da célula(intervalo)/condicional/célula/intervalo de comparação/adicionar</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -220,7 +343,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -257,12 +380,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -306,20 +447,11 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -336,11 +468,29 @@
     <xf numFmtId="4" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -656,11 +806,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BBD687A-3E64-44BC-B8CB-CC0BF0464A7B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,11 +825,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" s="4" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
       <c r="I1" s="5"/>
     </row>
     <row r="2" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -694,25 +844,25 @@
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="17" t="s">
         <v>5</v>
       </c>
     </row>
@@ -720,7 +870,9 @@
       <c r="B6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="15"/>
+      <c r="C6" s="27">
+        <v>17100</v>
+      </c>
       <c r="D6" s="9">
         <v>0.15</v>
       </c>
@@ -741,7 +893,9 @@
       <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="16"/>
+      <c r="C7" s="15">
+        <v>0</v>
+      </c>
       <c r="D7" s="10">
         <v>0.25</v>
       </c>
@@ -762,7 +916,9 @@
       <c r="B8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="16"/>
+      <c r="C8" s="15">
+        <v>4150</v>
+      </c>
       <c r="D8" s="10">
         <v>0.35</v>
       </c>
@@ -783,7 +939,9 @@
       <c r="B9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="17"/>
+      <c r="C9" s="28">
+        <v>1675</v>
+      </c>
       <c r="D9" s="11">
         <v>0.4</v>
       </c>
@@ -804,22 +962,37 @@
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22" t="s">
+      <c r="D11" s="19"/>
+      <c r="E11" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
+      <c r="F11" s="22">
+        <f>SUMPRODUCT($C$6:$C$9,F6:F9)</f>
+        <v>304.25</v>
+      </c>
+      <c r="G11" s="22">
+        <f t="shared" ref="G11:H11" si="0">SUMPRODUCT($C$6:$C$9,G6:G9)</f>
+        <v>650</v>
+      </c>
+      <c r="H11" s="22">
+        <f t="shared" si="0"/>
+        <v>783.25</v>
+      </c>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="24"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23" t="s">
+      <c r="B12" s="21">
+        <f>C6*D6+C7*D7+C8*D8+C9*D9</f>
+        <v>4687.5</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20" t="s">
         <v>13</v>
       </c>
       <c r="F12" s="11">
@@ -834,24 +1007,318 @@
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="21">
+        <f>SUMPRODUCT(C6:C9,D6:D9)</f>
+        <v>4687.5</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+    </row>
+    <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="2:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+    </row>
+    <row r="19" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B18:H18"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:I23"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:H16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3" max="8" width="13.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="1" customWidth="1"/>
+    <col min="11" max="18" width="15.7109375" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" s="4" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="27">
+        <v>17100</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0.15</v>
+      </c>
+      <c r="E6" s="14">
+        <v>17100</v>
+      </c>
+      <c r="F6" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="G6" s="9">
+        <v>0.02</v>
+      </c>
+      <c r="H6" s="9">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="15">
+        <v>0</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="E7" s="12">
+        <v>18900</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="G7" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="H7" s="10">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="15">
+        <v>4150</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0.35</v>
+      </c>
+      <c r="E8" s="12">
+        <v>4150</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="H8" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="28">
+        <v>1861</v>
+      </c>
+      <c r="D9" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="E9" s="13">
+        <v>16950</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="G9" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="H9" s="11">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="22">
+        <f>SUMPRODUCT($C$6:$C$9,F6:F9)</f>
+        <v>309.83</v>
+      </c>
+      <c r="G11" s="22">
+        <f t="shared" ref="G11:H11" si="0">SUMPRODUCT($C$6:$C$9,G6:G9)</f>
+        <v>661.16</v>
+      </c>
+      <c r="H11" s="22">
+        <f t="shared" si="0"/>
+        <v>799.99</v>
+      </c>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="21">
+        <f>C6*D6+C7*D7+C8*D8+C9*D9</f>
+        <v>4761.8999999999996</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="11">
+        <v>500</v>
+      </c>
+      <c r="G12" s="11">
+        <v>750</v>
+      </c>
+      <c r="H12" s="11">
+        <v>800</v>
+      </c>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="21">
+        <f>SUMPRODUCT(C6:C9,D6:D9)</f>
+        <v>4761.8999999999996</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+    </row>
+    <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="2:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+    </row>
+    <row r="19" spans="2:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+    </row>
+    <row r="20" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B19:H19"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>